<commit_message>
Added diagnosis and specialty variables
</commit_message>
<xml_diff>
--- a/Data/test-data.xlsx
+++ b/Data/test-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="23">
   <si>
     <t>date</t>
   </si>
@@ -46,6 +46,45 @@
   </si>
   <si>
     <t>OP</t>
+  </si>
+  <si>
+    <t>ep_icd10</t>
+  </si>
+  <si>
+    <t>A - head hurts</t>
+  </si>
+  <si>
+    <t>A - appendicitis</t>
+  </si>
+  <si>
+    <t>A - fractures in several areas</t>
+  </si>
+  <si>
+    <t>B- Sepsis</t>
+  </si>
+  <si>
+    <t>Specialty</t>
+  </si>
+  <si>
+    <t>Neurology</t>
+  </si>
+  <si>
+    <t>B - knee pain</t>
+  </si>
+  <si>
+    <t>Orthopaedics</t>
+  </si>
+  <si>
+    <t>Cardiology</t>
+  </si>
+  <si>
+    <t>Gastroenterology</t>
+  </si>
+  <si>
+    <t>Opthamology</t>
+  </si>
+  <si>
+    <t>General Surgery</t>
   </si>
 </sst>
 </file>
@@ -384,15 +423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C37"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,8 +441,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -414,7 +459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -424,8 +469,14 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -436,7 +487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -446,8 +497,14 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -458,7 +515,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>117</v>
       </c>
@@ -469,7 +526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>128</v>
       </c>
@@ -480,7 +537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>200</v>
       </c>
@@ -490,8 +547,11 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>299</v>
       </c>
@@ -501,8 +561,11 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>351</v>
       </c>
@@ -512,8 +575,11 @@
       <c r="C11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>21</v>
       </c>
@@ -524,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>42</v>
       </c>
@@ -534,8 +600,11 @@
       <c r="C13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>65</v>
       </c>
@@ -545,8 +614,11 @@
       <c r="C14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>70</v>
       </c>
@@ -557,7 +629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>93</v>
       </c>
@@ -567,8 +639,11 @@
       <c r="C16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>106</v>
       </c>
@@ -578,8 +653,14 @@
       <c r="C17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>107</v>
       </c>
@@ -590,7 +671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>120</v>
       </c>
@@ -601,7 +682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>151</v>
       </c>
@@ -612,7 +693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>159</v>
       </c>
@@ -622,8 +703,11 @@
       <c r="C21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>194</v>
       </c>
@@ -633,8 +717,11 @@
       <c r="C22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>211</v>
       </c>
@@ -644,8 +731,11 @@
       <c r="C23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>244</v>
       </c>
@@ -655,8 +745,11 @@
       <c r="C24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>263</v>
       </c>
@@ -666,8 +759,11 @@
       <c r="C25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>297</v>
       </c>
@@ -678,7 +774,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>298</v>
       </c>
@@ -688,8 +784,14 @@
       <c r="C27" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>299</v>
       </c>
@@ -700,7 +802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>300</v>
       </c>
@@ -711,7 +813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>301</v>
       </c>
@@ -721,8 +823,14 @@
       <c r="C30" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>301</v>
       </c>
@@ -733,7 +841,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>301</v>
       </c>
@@ -744,7 +852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>301</v>
       </c>
@@ -755,7 +863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>321</v>
       </c>
@@ -765,8 +873,11 @@
       <c r="C34" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>200</v>
       </c>
@@ -776,8 +887,11 @@
       <c r="C35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>117</v>
       </c>
@@ -787,8 +901,11 @@
       <c r="C36" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>177</v>
       </c>

</xml_diff>